<commit_message>
Began processing T0 clear plate data
The module I wrote proved to be really handy in abstracting and shortening the processing. I processed the long sample names and wells and added dry weight and treatment data already for T0 clear plate data. Now, I'm wrangling control readings.
</commit_message>
<xml_diff>
--- a/Metadata/2020-11-24-Plate-Layouts.xlsx
+++ b/Metadata/2020-11-24-Plate-Layouts.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B441DD-7F65-4C94-A17E-1DFFD5036148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BF271D-D47D-484F-8820-A4EAD37BB1F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Black plates (hydrolase)" sheetId="1" r:id="rId1"/>
     <sheet name="Clear plates (oxidase)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="90">
   <si>
     <t>A</t>
   </si>
@@ -236,9 +247,6 @@
     <t>Sample (Technical Replicate 2)</t>
   </si>
   <si>
-    <t>Highest concentration (uM)</t>
-  </si>
-  <si>
     <t>Highest substrate concentration (uM): 1 mg/7.9 mL</t>
   </si>
   <si>
@@ -288,6 +296,12 @@
   </si>
   <si>
     <t>pyrogallol 8 + H2O2</t>
+  </si>
+  <si>
+    <t>Highest concentration in wells (μM)</t>
+  </si>
+  <si>
+    <t>Highest concentration in reservoirs (μM)</t>
   </si>
 </sst>
 </file>
@@ -363,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +412,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -409,13 +432,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,8 +655,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1127,9 +1144,9 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>71</v>
+    <row r="11" spans="1:26" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="B11" s="2">
         <v>1000</v>
@@ -1175,17 +1192,40 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+    <row r="12" spans="1:26" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="2">
+        <f>B11/2</f>
+        <v>500</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:J12" si="0">C11/2</f>
+        <v>2000</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -28882,8 +28922,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28971,15 +29011,15 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>73</v>
+      <c r="B3" s="13" t="s">
+        <v>72</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>82</v>
+      <c r="C3" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>67</v>
@@ -28988,10 +29028,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>67</v>
@@ -29000,10 +29040,10 @@
         <v>10</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>67</v>
@@ -29025,15 +29065,15 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>74</v>
+      <c r="B4" s="13" t="s">
+        <v>73</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>81</v>
+      <c r="C4" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>67</v>
@@ -29042,10 +29082,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>67</v>
@@ -29054,10 +29094,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>67</v>
@@ -29079,15 +29119,15 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>75</v>
+      <c r="B5" s="13" t="s">
+        <v>74</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>83</v>
+      <c r="C5" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>67</v>
@@ -29096,10 +29136,10 @@
         <v>10</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>67</v>
@@ -29108,10 +29148,10 @@
         <v>10</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>67</v>
@@ -29133,15 +29173,15 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>76</v>
+      <c r="B6" s="13" t="s">
+        <v>75</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>84</v>
+      <c r="C6" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>67</v>
@@ -29150,10 +29190,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>67</v>
@@ -29162,10 +29202,10 @@
         <v>10</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>67</v>
@@ -29187,15 +29227,15 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>77</v>
+      <c r="B7" s="13" t="s">
+        <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>85</v>
+      <c r="C7" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>67</v>
@@ -29204,10 +29244,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>67</v>
@@ -29216,10 +29256,10 @@
         <v>10</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>67</v>
@@ -29241,15 +29281,15 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>78</v>
+      <c r="B8" s="13" t="s">
+        <v>77</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>86</v>
+      <c r="C8" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>67</v>
@@ -29258,10 +29298,10 @@
         <v>10</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>67</v>
@@ -29270,10 +29310,10 @@
         <v>10</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>67</v>
@@ -29295,15 +29335,15 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>79</v>
+      <c r="B9" s="13" t="s">
+        <v>78</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>87</v>
+      <c r="C9" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>67</v>
@@ -29312,10 +29352,10 @@
         <v>10</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>67</v>
@@ -29324,10 +29364,10 @@
         <v>10</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>67</v>
@@ -29349,15 +29389,15 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>80</v>
+      <c r="B10" s="13" t="s">
+        <v>79</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>88</v>
+      <c r="C10" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>67</v>
@@ -29366,10 +29406,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>67</v>
@@ -29378,10 +29418,10 @@
         <v>10</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>67</v>
@@ -29405,24 +29445,24 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="15" t="s">
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -29438,8 +29478,8 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>72</v>
+      <c r="A12" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>

</xml_diff>